<commit_message>
start submission main EDA notebook
</commit_message>
<xml_diff>
--- a/DataDictionary.xlsx
+++ b/DataDictionary.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shobh\Desktop\DSHS\homework1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776F289B-0DDB-4A01-8326-2773D2469B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC010608-B925-4E15-9392-E3D8B0CF15DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6284" yWindow="1702" windowWidth="18851" windowHeight="9962" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13929" tabRatio="622" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aggre" sheetId="12" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Aggre!$A$1:$B$331</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="572">
   <si>
     <t>IdControlVital</t>
   </si>
@@ -1697,6 +1711,45 @@
   </si>
   <si>
     <t>Cancellation Date</t>
+  </si>
+  <si>
+    <t>ComoSeEnteroCitaAg</t>
+  </si>
+  <si>
+    <t>FechaAlta</t>
+  </si>
+  <si>
+    <t>High Date</t>
+  </si>
+  <si>
+    <t>IdAgenda</t>
+  </si>
+  <si>
+    <t>Agenda ID</t>
+  </si>
+  <si>
+    <t>IdDeteccionMA</t>
+  </si>
+  <si>
+    <t>IdDeteccionRE</t>
+  </si>
+  <si>
+    <t>IdEstatusCita</t>
+  </si>
+  <si>
+    <t>Appointment Status</t>
+  </si>
+  <si>
+    <t>Referencia</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>Resultado</t>
+  </si>
+  <si>
+    <t>Outcome</t>
   </si>
 </sst>
 </file>
@@ -1772,7 +1825,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2106,11 +2170,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{292E9539-DDEC-46C1-BF61-190BF5D22634}">
-  <dimension ref="A1:B331"/>
+  <dimension ref="A1:B339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A306" workbookViewId="0">
-      <selection activeCell="A322" sqref="A322:B331"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05"/>
   <cols>
@@ -4766,7 +4828,74 @@
         <v>558</v>
       </c>
     </row>
+    <row r="332" spans="1:2">
+      <c r="A332" t="s">
+        <v>559</v>
+      </c>
+      <c r="B332" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2">
+      <c r="A333" t="s">
+        <v>560</v>
+      </c>
+      <c r="B333" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2">
+      <c r="A334" t="s">
+        <v>562</v>
+      </c>
+      <c r="B334" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2">
+      <c r="A335" t="s">
+        <v>564</v>
+      </c>
+      <c r="B335" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2">
+      <c r="A336" t="s">
+        <v>565</v>
+      </c>
+      <c r="B336" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2">
+      <c r="A337" t="s">
+        <v>566</v>
+      </c>
+      <c r="B337" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2">
+      <c r="A338" t="s">
+        <v>568</v>
+      </c>
+      <c r="B338" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2">
+      <c r="A339" t="s">
+        <v>570</v>
+      </c>
+      <c r="B339" t="s">
+        <v>571</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A332:A339">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>